<commit_message>
BIT emissions and leveling finished
</commit_message>
<xml_diff>
--- a/Cyberz/Montecarlo_Tokenomics/Results.xlsx
+++ b/Cyberz/Montecarlo_Tokenomics/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://puig-my.sharepoint.com/personal/pol_costas_puig_es/Documents/Escritorio/Python/General_Scripts/Personal/wip-codes/Cyberz/Montecarlo_Tokenomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="287" documentId="11_F25DC773A252ABDACC104865D99D76185BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B49651F7-A7BA-4134-A210-69C92D173FE2}"/>
+  <xr:revisionPtr revIDLastSave="293" documentId="11_F25DC773A252ABDACC104865D99D76185BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4D9DDE6-A2D6-431D-8C13-50A3E0592D19}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -218,10 +218,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1219,9 +1215,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -1230,7 +1223,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,27 +1906,27 @@
         <v>23</v>
       </c>
       <c r="E24">
-        <v>23215</v>
+        <v>25800</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>191025</v>
+        <v>193610</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="1"/>
-        <v>73.279671717171723</v>
+        <v>81.439393939393952</v>
       </c>
       <c r="H24" s="3">
         <f t="shared" si="2"/>
-        <v>602.98295454545462</v>
+        <v>611.1426767676769</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" si="3"/>
-        <v>18.319917929292931</v>
+        <v>20.359848484848488</v>
       </c>
       <c r="J24" s="2">
         <f t="shared" si="4"/>
-        <v>150.74573863636365</v>
+        <v>152.78566919191923</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1948,7 +1941,7 @@
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>219550</v>
+        <v>222135</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" si="1"/>
@@ -1956,7 +1949,7 @@
       </c>
       <c r="H25" s="3">
         <f t="shared" si="2"/>
-        <v>693.02398989898995</v>
+        <v>701.18371212121224</v>
       </c>
       <c r="I25" s="2">
         <f t="shared" si="3"/>
@@ -1964,7 +1957,7 @@
       </c>
       <c r="J25" s="2">
         <f t="shared" si="4"/>
-        <v>173.25599747474749</v>
+        <v>175.29592803030306</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1979,7 +1972,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>250950</v>
+        <v>253535</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" si="1"/>
@@ -1987,7 +1980,7 @@
       </c>
       <c r="H26" s="3">
         <f t="shared" si="2"/>
-        <v>792.14015151515162</v>
+        <v>800.2998737373739</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" si="3"/>
@@ -1995,13 +1988,14 @@
       </c>
       <c r="J26" s="2">
         <f t="shared" si="4"/>
-        <v>198.0350378787879</v>
+        <v>200.07496843434348</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId1"/>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
   </customProperties>
 </worksheet>
 </file>

</xml_diff>